<commit_message>
add seeds and suncoins accounts
</commit_message>
<xml_diff>
--- a/airdrop/suncoin.accounts.xlsx
+++ b/airdrop/suncoin.accounts.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suncoin.accounts" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="1683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="1705">
   <si>
     <t>Ty5PRjJhkcqTeGKQApJEz8wgcn7sbEG6ZT</t>
   </si>
@@ -5076,6 +5077,72 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>2JEc8JFzN2TGFy3wqeoe6eru3vwgq45sVSR</t>
+  </si>
+  <si>
+    <t>2TvPvWdA4zvaqpcwTfPLkgHGQtDAzdqQCb7</t>
+  </si>
+  <si>
+    <t>79xKvR3NQ7h4KD4vNt2PBLDtoKFDk1gG43</t>
+  </si>
+  <si>
+    <t>27CnhwPzuZV6zVh5Pe6JmM8HeFu35z3Jw8K</t>
+  </si>
+  <si>
+    <t>2M3pKMyx4NvfUFbWVvkT9Yv1STknFbL6VJp</t>
+  </si>
+  <si>
+    <t>agGeGte7zwoCKbQPQkd8L5dTKL49uLHYua</t>
+  </si>
+  <si>
+    <t>2GfRVqmmui6nddJkjjkjQ2fMbJFsWxezNV6</t>
+  </si>
+  <si>
+    <t>2Xvd17c6tVoJRfQ4npZWGjcz1LYrsqdYGXx</t>
+  </si>
+  <si>
+    <t>2Wgk1ghWPpD8NhZQi1ALbEKt8aNX9Np3Vim</t>
+  </si>
+  <si>
+    <t>2RDA7WebLA6unbyezKSNUoQvMDZZZWdQuzH</t>
+  </si>
+  <si>
+    <t>JSTLJ4FNxVwuhJdhBEvTVkwFWnqAhaDzic</t>
+  </si>
+  <si>
+    <t>2bcCTbYxByGXNAYNfSAVA759qsCXD15XApt</t>
+  </si>
+  <si>
+    <t>jRDhoRhcpmRHjgcF6Emn7Yuj3mHRGzm262</t>
+  </si>
+  <si>
+    <t>25T8PTJyLf6K4QisCZnv9J2EGLaramLt7fR</t>
+  </si>
+  <si>
+    <t>rXLbAYaGehJwzja7Gqkc3NHBi9hUmrAFDR</t>
+  </si>
+  <si>
+    <t>2S2Bfa4kvfauj2vWhhfbNRKwNLx5euxUBz5</t>
+  </si>
+  <si>
+    <t>5C1nVed6c9zqfSWDoHu7fmsEyUVXpyX8Cy</t>
+  </si>
+  <si>
+    <t>ZQ9QZRU1jGWRrXjGZWLdsZuqsQDa8BWWKo</t>
+  </si>
+  <si>
+    <t>YQtJPhqx6sAAQY6ePnsV1FzJm3vM9HC9Tz</t>
+  </si>
+  <si>
+    <t>rk973tk7wCJsRU9ExFHBKuPgvLeehjjRMy</t>
+  </si>
+  <si>
+    <t>PLUcUcFNSnK2rXoP2Fd5ugqGCMzn1ksfM1</t>
+  </si>
+  <si>
+    <t>Current balance</t>
   </si>
 </sst>
 </file>
@@ -5084,9 +5151,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5100,6 +5167,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF032F62"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5123,11 +5195,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5408,7 +5481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A1631" workbookViewId="0">
       <selection activeCell="B398" sqref="B398"/>
     </sheetView>
   </sheetViews>
@@ -23923,4 +23996,925 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B51" sqref="B2:B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B2" s="2">
+        <f>VLOOKUP(A2,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B3" s="2">
+        <f>VLOOKUP(A3,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B4" s="2">
+        <f>VLOOKUP(A4,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B5" s="2">
+        <f>VLOOKUP(A5,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B6" s="2">
+        <f>VLOOKUP(A6,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B7" s="2">
+        <f>VLOOKUP(A7,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B8" s="2">
+        <f>VLOOKUP(A8,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B9" s="2">
+        <f>VLOOKUP(A9,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B10" s="2">
+        <f>VLOOKUP(A10,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B11" s="2">
+        <f>VLOOKUP(A11,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B12" s="2">
+        <f>VLOOKUP(A12,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B13" s="2">
+        <f>VLOOKUP(A13,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B14" s="2">
+        <f>VLOOKUP(A14,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B15" s="2">
+        <f>VLOOKUP(A15,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B16" s="2">
+        <f>VLOOKUP(A16,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="B17" s="2">
+        <f>VLOOKUP(A17,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B18" s="2">
+        <f>VLOOKUP(A18,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B19" s="2">
+        <f>VLOOKUP(A19,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B20" s="2">
+        <f>VLOOKUP(A20,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B21" s="2">
+        <f>VLOOKUP(A21,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="2">
+        <f>VLOOKUP(A22,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="B23" s="2">
+        <f>VLOOKUP(A23,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2">
+        <f>VLOOKUP(A24,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="2">
+        <f>VLOOKUP(A25,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B26" s="2">
+        <f>VLOOKUP(A26,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B27" s="2">
+        <f>VLOOKUP(A27,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B28" s="2">
+        <f>VLOOKUP(A28,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="2">
+        <f>VLOOKUP(A29,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B30" s="2">
+        <f>VLOOKUP(A30,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <f>VLOOKUP(A31,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="B32" s="2">
+        <f>VLOOKUP(A32,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2">
+        <f>VLOOKUP(A33,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="B34" s="2">
+        <f>VLOOKUP(A34,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B35" s="2">
+        <f>VLOOKUP(A35,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="B36" s="2">
+        <f>VLOOKUP(A36,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="2">
+        <f>VLOOKUP(A37,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B38" s="2">
+        <f>VLOOKUP(A38,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B39" s="2">
+        <f>VLOOKUP(A39,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="B40" s="2">
+        <f>VLOOKUP(A40,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41" s="2">
+        <f>VLOOKUP(A41,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B42" s="2">
+        <f>VLOOKUP(A42,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" s="2">
+        <f>VLOOKUP(A43,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B44" s="2">
+        <f>VLOOKUP(A44,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B45" s="2">
+        <f>VLOOKUP(A45,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="B46" s="2">
+        <f>VLOOKUP(A46,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B47" s="2">
+        <f>VLOOKUP(A47,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B48" s="2">
+        <f>VLOOKUP(A48,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="B49" s="2">
+        <f>VLOOKUP(A49,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B50" s="2">
+        <f>VLOOKUP(A50,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B51" s="2">
+        <f>VLOOKUP(A51,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B52" s="2">
+        <f>VLOOKUP(A52,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B53" s="2">
+        <f>VLOOKUP(A53,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B54" s="2">
+        <f>VLOOKUP(A54,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="2">
+        <f>VLOOKUP(A55,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="2">
+        <f>VLOOKUP(A56,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="B57" s="2">
+        <f>VLOOKUP(A57,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B58" s="2">
+        <f>VLOOKUP(A58,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="B59" s="2">
+        <f>VLOOKUP(A59,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B60" s="2">
+        <f>VLOOKUP(A60,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B61" s="2">
+        <f>VLOOKUP(A61,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B62" s="2">
+        <f>VLOOKUP(A62,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B63" s="2">
+        <f>VLOOKUP(A63,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B64" s="2">
+        <f>VLOOKUP(A64,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B65" s="2">
+        <f>VLOOKUP(A65,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="B66" s="2">
+        <f>VLOOKUP(A66,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B67" s="2">
+        <f>VLOOKUP(A67,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="B68" s="2">
+        <f>VLOOKUP(A68,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B69" s="2">
+        <f>VLOOKUP(A69,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B70" s="2">
+        <f>VLOOKUP(A70,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B71" s="2">
+        <f>VLOOKUP(A71,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B72" s="2">
+        <f>VLOOKUP(A72,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B73" s="2">
+        <f>VLOOKUP(A73,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="B74" s="2">
+        <f>VLOOKUP(A74,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9.6029999999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B75" s="2">
+        <f>VLOOKUP(A75,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B76" s="2">
+        <f>VLOOKUP(A76,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="B77" s="2">
+        <f>VLOOKUP(A77,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B78" s="2">
+        <f>VLOOKUP(A78,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B79" s="2">
+        <f>VLOOKUP(A79,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="B80" s="2">
+        <f>VLOOKUP(A80,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B81" s="2">
+        <f>VLOOKUP(A81,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B82" s="2">
+        <f>VLOOKUP(A82,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B83" s="2">
+        <f>VLOOKUP(A83,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="B84" s="2">
+        <f>VLOOKUP(A84,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B85" s="2">
+        <f>VLOOKUP(A85,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B86" s="2">
+        <f>VLOOKUP(A86,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B87" s="2">
+        <f>VLOOKUP(A87,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B88" s="2">
+        <f>VLOOKUP(A88,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="B89" s="2">
+        <f>VLOOKUP(A89,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B90" s="2">
+        <f>VLOOKUP(A90,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B91" s="2">
+        <f>VLOOKUP(A91,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B92" s="2">
+        <f>VLOOKUP(A92,suncoin.accounts!$B$2:$C$1681, 2, TRUE)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>823</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B101">
+    <sortCondition descending="1" ref="B2:B101"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>